<commit_message>
data wrangling - finding meaningful relationships to pursue further
</commit_message>
<xml_diff>
--- a/data/nh_to_cluster.xlsx
+++ b/data/nh_to_cluster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renudinesh/Final-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BCF4BE-033A-F541-9DED-09C824438C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1814F314-BA56-AF4A-8465-94664CDE1533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,9 +505,6 @@
     <t>North Scarborough &amp; South Scarborough</t>
   </si>
   <si>
-    <t>North Etobicoke &amp; South Etobiceto</t>
-  </si>
-  <si>
     <t>Toronto</t>
   </si>
   <si>
@@ -521,6 +518,9 @@
   </si>
   <si>
     <t>Downtown East &amp; Downtown West</t>
+  </si>
+  <si>
+    <t>North Etobicoke &amp; South Etobicoke</t>
   </si>
 </sst>
 </file>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="174" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="174" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -930,7 +930,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -938,7 +938,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -946,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -954,7 +954,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -962,7 +962,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -970,7 +970,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -978,7 +978,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -986,7 +986,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -994,7 +994,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1002,7 +1002,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1034,7 +1034,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1050,7 +1050,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1058,7 +1058,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1066,7 +1066,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1074,7 +1074,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1082,7 +1082,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1090,7 +1090,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1098,7 +1098,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1130,7 +1130,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1146,7 +1146,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1154,7 +1154,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1162,7 +1162,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1170,7 +1170,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1186,7 +1186,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1194,7 +1194,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1202,7 +1202,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1234,7 +1234,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1242,7 +1242,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1258,7 +1258,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1266,7 +1266,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1274,7 +1274,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1282,7 +1282,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1290,7 +1290,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1298,7 +1298,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1314,7 +1314,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1322,7 +1322,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1330,7 +1330,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1338,7 +1338,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1354,7 +1354,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1370,7 +1370,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1378,7 +1378,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -1386,7 +1386,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1394,7 +1394,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -1410,7 +1410,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1418,7 +1418,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -1426,7 +1426,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -1434,7 +1434,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -1442,7 +1442,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -1450,7 +1450,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -1466,7 +1466,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -1474,7 +1474,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1482,7 +1482,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -1490,7 +1490,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1506,7 +1506,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1514,7 +1514,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1522,7 +1522,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -1538,7 +1538,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1546,7 +1546,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1554,7 +1554,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -1562,7 +1562,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -1570,7 +1570,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1578,7 +1578,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -1586,7 +1586,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -1610,7 +1610,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -1618,7 +1618,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -1634,7 +1634,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -1658,7 +1658,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -1666,7 +1666,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -1674,7 +1674,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -1682,7 +1682,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -1690,7 +1690,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -1698,7 +1698,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -1706,7 +1706,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -1714,7 +1714,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -1722,7 +1722,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -1730,7 +1730,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -1738,7 +1738,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -1762,7 +1762,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -1770,7 +1770,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -1778,7 +1778,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -1786,7 +1786,7 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -1794,7 +1794,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -1802,7 +1802,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -1810,7 +1810,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -1818,7 +1818,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
@@ -1826,7 +1826,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -1834,7 +1834,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
@@ -1842,7 +1842,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -1850,7 +1850,7 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
@@ -1858,7 +1858,7 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
@@ -1866,7 +1866,7 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
@@ -1874,7 +1874,7 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
@@ -1890,7 +1890,7 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
@@ -1898,7 +1898,7 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
@@ -1906,7 +1906,7 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
@@ -1914,7 +1914,7 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
@@ -1922,7 +1922,7 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
@@ -1930,7 +1930,7 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -1938,7 +1938,7 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
@@ -1954,7 +1954,7 @@
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
@@ -1962,7 +1962,7 @@
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -1970,7 +1970,7 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -1978,7 +1978,7 @@
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
@@ -1986,7 +1986,7 @@
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -1994,7 +1994,7 @@
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
@@ -2002,7 +2002,7 @@
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -2010,7 +2010,7 @@
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
@@ -2026,7 +2026,7 @@
         <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
@@ -2034,7 +2034,7 @@
         <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
@@ -2050,7 +2050,7 @@
         <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
@@ -2058,7 +2058,7 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
@@ -2066,7 +2066,7 @@
         <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
@@ -2082,7 +2082,7 @@
         <v>148</v>
       </c>
       <c r="B148" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
@@ -2090,7 +2090,7 @@
         <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
@@ -2106,7 +2106,7 @@
         <v>151</v>
       </c>
       <c r="B151" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
@@ -2114,7 +2114,7 @@
         <v>152</v>
       </c>
       <c r="B152" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
@@ -2122,7 +2122,7 @@
         <v>153</v>
       </c>
       <c r="B153" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
@@ -2130,7 +2130,7 @@
         <v>154</v>
       </c>
       <c r="B154" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
@@ -2138,7 +2138,7 @@
         <v>155</v>
       </c>
       <c r="B155" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
@@ -2146,7 +2146,7 @@
         <v>156</v>
       </c>
       <c r="B156" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
@@ -2154,7 +2154,7 @@
         <v>157</v>
       </c>
       <c r="B157" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
@@ -2162,7 +2162,7 @@
         <v>158</v>
       </c>
       <c r="B158" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
@@ -2170,7 +2170,7 @@
         <v>159</v>
       </c>
       <c r="B159" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>